<commit_message>
changed chellanges db version day 1 fix
</commit_message>
<xml_diff>
--- a/convert/together23_pieces_datenbank.xlsx
+++ b/convert/together23_pieces_datenbank.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26803"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26803"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ooepp.sharepoint.com/sites/Landeslager2023/Freigegebene Dokumente/General/CaEx/Programm/Challenges/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF561980-1328-49A0-ADBE-EC91FD964C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D52087B-267F-434C-94ED-12420CB10914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="27288" windowHeight="17544" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="27288" windowHeight="17544" firstSheet="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Aufgabenkatalog" sheetId="1" r:id="rId1"/>
@@ -3609,10 +3609,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AV333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="C334" sqref="C334"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="C137" sqref="C137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -3711,7 +3712,7 @@
       <c r="AU1" s="118"/>
       <c r="AV1" s="118"/>
     </row>
-    <row r="2" spans="1:48" ht="15.6">
+    <row r="2" spans="1:48" ht="15.6" hidden="1">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3785,7 +3786,7 @@
       <c r="AU2" s="1"/>
       <c r="AV2" s="1"/>
     </row>
-    <row r="3" spans="1:48" s="51" customFormat="1" ht="15">
+    <row r="3" spans="1:48" s="51" customFormat="1" ht="15" hidden="1">
       <c r="A3" s="51">
         <v>2</v>
       </c>
@@ -3861,7 +3862,7 @@
       <c r="AU3" s="50"/>
       <c r="AV3" s="50"/>
     </row>
-    <row r="4" spans="1:48" ht="15.6">
+    <row r="4" spans="1:48" ht="15.6" hidden="1">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3935,7 +3936,7 @@
       <c r="AU4" s="1"/>
       <c r="AV4" s="1"/>
     </row>
-    <row r="5" spans="1:48" ht="15.6">
+    <row r="5" spans="1:48" ht="15.6" hidden="1">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4083,7 +4084,7 @@
       <c r="AU6" s="1"/>
       <c r="AV6" s="1"/>
     </row>
-    <row r="7" spans="1:48" ht="15.6">
+    <row r="7" spans="1:48" ht="15.6" hidden="1">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4157,7 +4158,7 @@
       <c r="AU7" s="1"/>
       <c r="AV7" s="1"/>
     </row>
-    <row r="8" spans="1:48" ht="15.6">
+    <row r="8" spans="1:48" ht="15.6" hidden="1">
       <c r="A8" s="51">
         <v>7</v>
       </c>
@@ -4231,7 +4232,7 @@
       <c r="AU8" s="1"/>
       <c r="AV8" s="1"/>
     </row>
-    <row r="9" spans="1:48" s="31" customFormat="1" ht="15">
+    <row r="9" spans="1:48" s="31" customFormat="1" ht="15" hidden="1">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4303,7 +4304,7 @@
       <c r="AU9" s="30"/>
       <c r="AV9" s="30"/>
     </row>
-    <row r="10" spans="1:48" ht="15.6">
+    <row r="10" spans="1:48" ht="15.6" hidden="1">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4379,7 +4380,7 @@
       <c r="AU10" s="1"/>
       <c r="AV10" s="1"/>
     </row>
-    <row r="11" spans="1:48" s="31" customFormat="1" ht="15">
+    <row r="11" spans="1:48" s="31" customFormat="1" ht="15" hidden="1">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4675,7 +4676,7 @@
       <c r="AU14" s="1"/>
       <c r="AV14" s="1"/>
     </row>
-    <row r="15" spans="1:48" ht="15.6">
+    <row r="15" spans="1:48" ht="15.6" hidden="1">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4749,7 +4750,7 @@
       <c r="AU15" s="1"/>
       <c r="AV15" s="1"/>
     </row>
-    <row r="16" spans="1:48" ht="15.6">
+    <row r="16" spans="1:48" ht="15.6" hidden="1">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4897,7 +4898,7 @@
       <c r="AU17" s="1"/>
       <c r="AV17" s="1"/>
     </row>
-    <row r="18" spans="1:48" ht="15.6">
+    <row r="18" spans="1:48" ht="15.6" hidden="1">
       <c r="A18" s="51">
         <v>17</v>
       </c>
@@ -4981,7 +4982,7 @@
         <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D19" s="20" t="s">
         <v>16</v>
@@ -5193,7 +5194,7 @@
       <c r="AU21" s="1"/>
       <c r="AV21" s="1"/>
     </row>
-    <row r="22" spans="1:48" s="31" customFormat="1" ht="15">
+    <row r="22" spans="1:48" s="31" customFormat="1" ht="15" hidden="1">
       <c r="A22">
         <v>21</v>
       </c>
@@ -5267,7 +5268,7 @@
       <c r="AU22" s="30"/>
       <c r="AV22" s="30"/>
     </row>
-    <row r="23" spans="1:48" ht="15.6">
+    <row r="23" spans="1:48" ht="15.6" hidden="1">
       <c r="A23" s="51">
         <v>22</v>
       </c>
@@ -5341,7 +5342,7 @@
       <c r="AU23" s="1"/>
       <c r="AV23" s="1"/>
     </row>
-    <row r="24" spans="1:48" ht="15.6">
+    <row r="24" spans="1:48" ht="15.6" hidden="1">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5415,7 +5416,7 @@
       <c r="AU24" s="1"/>
       <c r="AV24" s="1"/>
     </row>
-    <row r="25" spans="1:48" ht="15.6">
+    <row r="25" spans="1:48" ht="15.6" hidden="1">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5497,7 +5498,7 @@
         <v>128</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D26" s="17" t="s">
         <v>16</v>
@@ -5563,7 +5564,7 @@
       <c r="AU26" s="1"/>
       <c r="AV26" s="1"/>
     </row>
-    <row r="27" spans="1:48" ht="15.6">
+    <row r="27" spans="1:48" ht="15.6" hidden="1">
       <c r="A27">
         <v>26</v>
       </c>
@@ -5637,7 +5638,7 @@
       <c r="AU27" s="1"/>
       <c r="AV27" s="1"/>
     </row>
-    <row r="28" spans="1:48" ht="15.6">
+    <row r="28" spans="1:48" ht="15.6" hidden="1">
       <c r="A28" s="51">
         <v>27</v>
       </c>
@@ -5711,7 +5712,7 @@
       <c r="AU28" s="1"/>
       <c r="AV28" s="1"/>
     </row>
-    <row r="29" spans="1:48" ht="15.6">
+    <row r="29" spans="1:48" ht="15.6" hidden="1">
       <c r="A29">
         <v>28</v>
       </c>
@@ -5785,7 +5786,7 @@
       <c r="AU29" s="1"/>
       <c r="AV29" s="1"/>
     </row>
-    <row r="30" spans="1:48" s="51" customFormat="1" ht="15">
+    <row r="30" spans="1:48" s="51" customFormat="1" ht="15" hidden="1">
       <c r="A30">
         <v>29</v>
       </c>
@@ -5867,7 +5868,7 @@
         <v>128</v>
       </c>
       <c r="C31" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D31" s="17" t="s">
         <v>16</v>
@@ -5933,7 +5934,7 @@
       <c r="AU31" s="1"/>
       <c r="AV31" s="1"/>
     </row>
-    <row r="32" spans="1:48" ht="15.6">
+    <row r="32" spans="1:48" ht="15.6" hidden="1">
       <c r="A32">
         <v>31</v>
       </c>
@@ -6015,7 +6016,7 @@
         <v>128</v>
       </c>
       <c r="C33" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D33" s="20" t="s">
         <v>16</v>
@@ -6155,7 +6156,7 @@
       <c r="AU34" s="1"/>
       <c r="AV34" s="1"/>
     </row>
-    <row r="35" spans="1:48" ht="15.6">
+    <row r="35" spans="1:48" ht="15.6" hidden="1">
       <c r="A35">
         <v>34</v>
       </c>
@@ -6237,7 +6238,7 @@
         <v>128</v>
       </c>
       <c r="C36" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D36" s="86" t="s">
         <v>16</v>
@@ -6305,7 +6306,7 @@
       <c r="AU36" s="92"/>
       <c r="AV36" s="92"/>
     </row>
-    <row r="37" spans="1:48" ht="15.6">
+    <row r="37" spans="1:48" ht="15.6" hidden="1">
       <c r="A37">
         <v>36</v>
       </c>
@@ -6381,7 +6382,7 @@
       <c r="AU37" s="1"/>
       <c r="AV37" s="1"/>
     </row>
-    <row r="38" spans="1:48" ht="15.6">
+    <row r="38" spans="1:48" ht="15.6" hidden="1">
       <c r="A38" s="51">
         <v>37</v>
       </c>
@@ -6457,7 +6458,7 @@
       <c r="AU38" s="1"/>
       <c r="AV38" s="1"/>
     </row>
-    <row r="39" spans="1:48" ht="15.6">
+    <row r="39" spans="1:48" ht="15.6" hidden="1">
       <c r="A39">
         <v>38</v>
       </c>
@@ -6531,7 +6532,7 @@
       <c r="AU39" s="1"/>
       <c r="AV39" s="1"/>
     </row>
-    <row r="40" spans="1:48" ht="15.6">
+    <row r="40" spans="1:48" ht="15.6" hidden="1">
       <c r="A40">
         <v>39</v>
       </c>
@@ -6679,7 +6680,7 @@
       <c r="AU41" s="1"/>
       <c r="AV41" s="1"/>
     </row>
-    <row r="42" spans="1:48" ht="15.6">
+    <row r="42" spans="1:48" ht="15.6" hidden="1">
       <c r="A42">
         <v>41</v>
       </c>
@@ -6753,7 +6754,7 @@
       <c r="AU42" s="1"/>
       <c r="AV42" s="1"/>
     </row>
-    <row r="43" spans="1:48" ht="15.6">
+    <row r="43" spans="1:48" ht="15.6" hidden="1">
       <c r="A43" s="51">
         <v>42</v>
       </c>
@@ -6827,7 +6828,7 @@
       <c r="AU43" s="1"/>
       <c r="AV43" s="1"/>
     </row>
-    <row r="44" spans="1:48" ht="15.6">
+    <row r="44" spans="1:48" ht="15.6" hidden="1">
       <c r="A44">
         <v>43</v>
       </c>
@@ -6901,7 +6902,7 @@
       <c r="AU44" s="1"/>
       <c r="AV44" s="1"/>
     </row>
-    <row r="45" spans="1:48" ht="15.6">
+    <row r="45" spans="1:48" ht="15.6" hidden="1">
       <c r="A45">
         <v>44</v>
       </c>
@@ -6975,7 +6976,7 @@
       <c r="AU45" s="1"/>
       <c r="AV45" s="1"/>
     </row>
-    <row r="46" spans="1:48" ht="15.6">
+    <row r="46" spans="1:48" ht="15.6" hidden="1">
       <c r="A46">
         <v>45</v>
       </c>
@@ -7123,7 +7124,7 @@
       <c r="AU47" s="1"/>
       <c r="AV47" s="1"/>
     </row>
-    <row r="48" spans="1:48" ht="15.6">
+    <row r="48" spans="1:48" ht="15.6" hidden="1">
       <c r="A48" s="51">
         <v>47</v>
       </c>
@@ -7271,7 +7272,7 @@
       <c r="AU49" s="1"/>
       <c r="AV49" s="1"/>
     </row>
-    <row r="50" spans="1:48" s="85" customFormat="1" ht="15">
+    <row r="50" spans="1:48" s="85" customFormat="1" ht="15" hidden="1">
       <c r="A50">
         <v>49</v>
       </c>
@@ -7345,7 +7346,7 @@
       <c r="AU50" s="92"/>
       <c r="AV50" s="92"/>
     </row>
-    <row r="51" spans="1:48" s="31" customFormat="1" ht="15">
+    <row r="51" spans="1:48" s="31" customFormat="1" ht="15" hidden="1">
       <c r="A51">
         <v>50</v>
       </c>
@@ -7417,7 +7418,7 @@
       <c r="AU51" s="30"/>
       <c r="AV51" s="30"/>
     </row>
-    <row r="52" spans="1:48" ht="15.6">
+    <row r="52" spans="1:48" ht="15.6" hidden="1">
       <c r="A52">
         <v>51</v>
       </c>
@@ -7491,7 +7492,7 @@
       <c r="AU52" s="1"/>
       <c r="AV52" s="1"/>
     </row>
-    <row r="53" spans="1:48" ht="15">
+    <row r="53" spans="1:48" ht="15" hidden="1">
       <c r="A53" s="51">
         <v>52</v>
       </c>
@@ -7567,7 +7568,7 @@
       <c r="AU53" s="1"/>
       <c r="AV53" s="1"/>
     </row>
-    <row r="54" spans="1:48" s="31" customFormat="1" ht="15">
+    <row r="54" spans="1:48" s="31" customFormat="1" ht="15" hidden="1">
       <c r="A54">
         <v>53</v>
       </c>
@@ -7639,7 +7640,7 @@
       <c r="AU54" s="30"/>
       <c r="AV54" s="30"/>
     </row>
-    <row r="55" spans="1:48" ht="15.6">
+    <row r="55" spans="1:48" ht="15.6" hidden="1">
       <c r="A55">
         <v>54</v>
       </c>
@@ -7789,7 +7790,7 @@
       <c r="AU56" s="1"/>
       <c r="AV56" s="1"/>
     </row>
-    <row r="57" spans="1:48" s="27" customFormat="1" ht="15">
+    <row r="57" spans="1:48" s="27" customFormat="1" ht="15" hidden="1">
       <c r="A57">
         <v>56</v>
       </c>
@@ -7861,7 +7862,7 @@
       <c r="AU57" s="26"/>
       <c r="AV57" s="26"/>
     </row>
-    <row r="58" spans="1:48" s="51" customFormat="1" ht="15">
+    <row r="58" spans="1:48" s="51" customFormat="1" ht="15" hidden="1">
       <c r="A58" s="51">
         <v>57</v>
       </c>
@@ -8009,7 +8010,7 @@
       <c r="AU59" s="1"/>
       <c r="AV59" s="1"/>
     </row>
-    <row r="60" spans="1:48" ht="15.6">
+    <row r="60" spans="1:48" ht="15.6" hidden="1">
       <c r="A60">
         <v>59</v>
       </c>
@@ -8083,7 +8084,7 @@
       <c r="AU60" s="1"/>
       <c r="AV60" s="1"/>
     </row>
-    <row r="61" spans="1:48" ht="15.6">
+    <row r="61" spans="1:48" ht="15.6" hidden="1">
       <c r="A61">
         <v>60</v>
       </c>
@@ -8157,7 +8158,7 @@
       <c r="AU61" s="1"/>
       <c r="AV61" s="1"/>
     </row>
-    <row r="62" spans="1:48" ht="15.6">
+    <row r="62" spans="1:48" ht="15.6" hidden="1">
       <c r="A62">
         <v>61</v>
       </c>
@@ -8231,7 +8232,7 @@
       <c r="AU62" s="1"/>
       <c r="AV62" s="1"/>
     </row>
-    <row r="63" spans="1:48" ht="15.6">
+    <row r="63" spans="1:48" ht="15.6" hidden="1">
       <c r="A63" s="51">
         <v>62</v>
       </c>
@@ -8379,7 +8380,7 @@
       <c r="AU64" s="1"/>
       <c r="AV64" s="1"/>
     </row>
-    <row r="65" spans="1:48" ht="15.6">
+    <row r="65" spans="1:48" ht="15.6" hidden="1">
       <c r="A65">
         <v>64</v>
       </c>
@@ -8453,7 +8454,7 @@
       <c r="AU65" s="1"/>
       <c r="AV65" s="1"/>
     </row>
-    <row r="66" spans="1:48" ht="15.6">
+    <row r="66" spans="1:48" ht="15.6" hidden="1">
       <c r="A66">
         <v>65</v>
       </c>
@@ -8527,7 +8528,7 @@
       <c r="AU66" s="1"/>
       <c r="AV66" s="1"/>
     </row>
-    <row r="67" spans="1:48" ht="15.6">
+    <row r="67" spans="1:48" ht="15.6" hidden="1">
       <c r="A67">
         <v>66</v>
       </c>
@@ -8601,7 +8602,7 @@
       <c r="AU67" s="1"/>
       <c r="AV67" s="1"/>
     </row>
-    <row r="68" spans="1:48" s="31" customFormat="1" ht="15">
+    <row r="68" spans="1:48" s="31" customFormat="1" ht="15" hidden="1">
       <c r="A68" s="51">
         <v>67</v>
       </c>
@@ -8823,7 +8824,7 @@
       <c r="AU70" s="1"/>
       <c r="AV70" s="1"/>
     </row>
-    <row r="71" spans="1:48" ht="15.6">
+    <row r="71" spans="1:48" ht="15.6" hidden="1">
       <c r="A71">
         <v>70</v>
       </c>
@@ -8899,7 +8900,7 @@
       <c r="AU71" s="1"/>
       <c r="AV71" s="1"/>
     </row>
-    <row r="72" spans="1:48" s="31" customFormat="1" ht="15">
+    <row r="72" spans="1:48" s="31" customFormat="1" ht="15" hidden="1">
       <c r="A72">
         <v>71</v>
       </c>
@@ -8979,7 +8980,7 @@
         <v>238</v>
       </c>
       <c r="C73" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D73" s="20" t="s">
         <v>16</v>
@@ -9043,7 +9044,7 @@
       <c r="AU73" s="30"/>
       <c r="AV73" s="30"/>
     </row>
-    <row r="74" spans="1:48" s="31" customFormat="1" ht="15">
+    <row r="74" spans="1:48" s="31" customFormat="1" ht="15" hidden="1">
       <c r="A74">
         <v>73</v>
       </c>
@@ -9123,7 +9124,7 @@
         <v>238</v>
       </c>
       <c r="C75" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D75" s="20" t="s">
         <v>16</v>
@@ -9193,7 +9194,7 @@
         <v>238</v>
       </c>
       <c r="C76" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D76" s="20" t="s">
         <v>16</v>
@@ -9263,7 +9264,7 @@
         <v>238</v>
       </c>
       <c r="C77" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D77" s="20" t="s">
         <v>16</v>
@@ -9333,7 +9334,7 @@
         <v>238</v>
       </c>
       <c r="C78" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D78" s="20" t="s">
         <v>16</v>
@@ -9403,7 +9404,7 @@
         <v>238</v>
       </c>
       <c r="C79" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D79" s="20" t="s">
         <v>16</v>
@@ -9617,7 +9618,7 @@
         <v>363</v>
       </c>
       <c r="C82" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D82" s="17" t="s">
         <v>75</v>
@@ -9683,7 +9684,7 @@
       <c r="AU82" s="1"/>
       <c r="AV82" s="1"/>
     </row>
-    <row r="83" spans="1:48" ht="15">
+    <row r="83" spans="1:48" ht="15" hidden="1">
       <c r="A83" s="51">
         <v>82</v>
       </c>
@@ -9755,7 +9756,7 @@
       <c r="AU83" s="1"/>
       <c r="AV83" s="1"/>
     </row>
-    <row r="84" spans="1:48" ht="15.6">
+    <row r="84" spans="1:48" ht="15.6" hidden="1">
       <c r="A84">
         <v>83</v>
       </c>
@@ -9983,7 +9984,7 @@
         <v>363</v>
       </c>
       <c r="C87" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D87" s="17" t="s">
         <v>75</v>
@@ -10057,7 +10058,7 @@
         <v>363</v>
       </c>
       <c r="C88" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D88" s="17" t="s">
         <v>75</v>
@@ -10129,7 +10130,7 @@
         <v>363</v>
       </c>
       <c r="C89" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D89" s="17" t="s">
         <v>75</v>
@@ -10277,7 +10278,7 @@
         <v>363</v>
       </c>
       <c r="C91" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D91" s="17" t="s">
         <v>75</v>
@@ -10351,7 +10352,7 @@
         <v>363</v>
       </c>
       <c r="C92" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D92" s="17" t="s">
         <v>75</v>
@@ -10495,7 +10496,7 @@
         <v>363</v>
       </c>
       <c r="C94" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D94" s="17" t="s">
         <v>75</v>
@@ -10789,7 +10790,7 @@
         <v>363</v>
       </c>
       <c r="C98" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D98" s="86" t="s">
         <v>75</v>
@@ -10861,7 +10862,7 @@
         <v>363</v>
       </c>
       <c r="C99" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D99" s="17" t="s">
         <v>75</v>
@@ -11079,7 +11080,7 @@
         <v>363</v>
       </c>
       <c r="C102" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D102" s="86" t="s">
         <v>75</v>
@@ -11151,7 +11152,7 @@
         <v>363</v>
       </c>
       <c r="C103" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D103" s="17" t="s">
         <v>75</v>
@@ -11215,7 +11216,7 @@
       <c r="AU103" s="1"/>
       <c r="AV103" s="1"/>
     </row>
-    <row r="104" spans="1:48" ht="15.6">
+    <row r="104" spans="1:48" ht="15.6" hidden="1">
       <c r="A104">
         <v>103</v>
       </c>
@@ -11289,7 +11290,7 @@
       <c r="AU104" s="1"/>
       <c r="AV104" s="1"/>
     </row>
-    <row r="105" spans="1:48" ht="15.6">
+    <row r="105" spans="1:48" ht="15.6" hidden="1">
       <c r="A105">
         <v>104</v>
       </c>
@@ -11363,7 +11364,7 @@
       <c r="AU105" s="1"/>
       <c r="AV105" s="1"/>
     </row>
-    <row r="106" spans="1:48" ht="15.6">
+    <row r="106" spans="1:48" ht="15.6" hidden="1">
       <c r="A106">
         <v>105</v>
       </c>
@@ -11437,7 +11438,7 @@
       <c r="AU106" s="1"/>
       <c r="AV106" s="1"/>
     </row>
-    <row r="107" spans="1:48" ht="15.6">
+    <row r="107" spans="1:48" ht="15.6" hidden="1">
       <c r="A107">
         <v>106</v>
       </c>
@@ -11511,7 +11512,7 @@
       <c r="AU107" s="1"/>
       <c r="AV107" s="1"/>
     </row>
-    <row r="108" spans="1:48" ht="15.6">
+    <row r="108" spans="1:48" ht="15.6" hidden="1">
       <c r="A108" s="51">
         <v>107</v>
       </c>
@@ -11585,7 +11586,7 @@
       <c r="AU108" s="1"/>
       <c r="AV108" s="1"/>
     </row>
-    <row r="109" spans="1:48" ht="15.6">
+    <row r="109" spans="1:48" ht="15.6" hidden="1">
       <c r="A109">
         <v>108</v>
       </c>
@@ -11659,7 +11660,7 @@
       <c r="AU109" s="1"/>
       <c r="AV109" s="1"/>
     </row>
-    <row r="110" spans="1:48" ht="15">
+    <row r="110" spans="1:48" ht="15" hidden="1">
       <c r="A110">
         <v>109</v>
       </c>
@@ -11743,7 +11744,7 @@
         <v>359</v>
       </c>
       <c r="C111" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D111" s="75" t="s">
         <v>75</v>
@@ -11816,7 +11817,7 @@
         <v>359</v>
       </c>
       <c r="C112" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D112" s="75" t="s">
         <v>75</v>
@@ -11889,7 +11890,7 @@
         <v>359</v>
       </c>
       <c r="C113" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D113" s="75" t="s">
         <v>75</v>
@@ -11954,7 +11955,7 @@
       <c r="AU113" s="83"/>
       <c r="AV113" s="83"/>
     </row>
-    <row r="114" spans="1:48" ht="15.6">
+    <row r="114" spans="1:48" ht="15.6" hidden="1">
       <c r="A114">
         <v>113</v>
       </c>
@@ -12028,7 +12029,7 @@
       <c r="AU114" s="1"/>
       <c r="AV114" s="1"/>
     </row>
-    <row r="115" spans="1:48" ht="15.6">
+    <row r="115" spans="1:48" ht="15.6" hidden="1">
       <c r="A115">
         <v>114</v>
       </c>
@@ -12180,7 +12181,7 @@
       <c r="AU116" s="1"/>
       <c r="AV116" s="1"/>
     </row>
-    <row r="117" spans="1:48" ht="15.6">
+    <row r="117" spans="1:48" ht="15.6" hidden="1">
       <c r="A117">
         <v>116</v>
       </c>
@@ -12254,7 +12255,7 @@
       <c r="AU117" s="1"/>
       <c r="AV117" s="1"/>
     </row>
-    <row r="118" spans="1:48" ht="15.6">
+    <row r="118" spans="1:48" ht="15.6" hidden="1">
       <c r="A118" s="51">
         <v>117</v>
       </c>
@@ -12336,7 +12337,7 @@
         <v>359</v>
       </c>
       <c r="C119" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D119" s="17" t="s">
         <v>75</v>
@@ -12410,7 +12411,7 @@
         <v>359</v>
       </c>
       <c r="C120" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D120" s="86" t="s">
         <v>75</v>
@@ -12477,7 +12478,7 @@
       <c r="AU120" s="92"/>
       <c r="AV120" s="92"/>
     </row>
-    <row r="121" spans="1:48" ht="15.6">
+    <row r="121" spans="1:48" ht="15.6" hidden="1">
       <c r="A121">
         <v>120</v>
       </c>
@@ -12625,7 +12626,7 @@
       <c r="AU122" s="1"/>
       <c r="AV122" s="1"/>
     </row>
-    <row r="123" spans="1:48" ht="15.6">
+    <row r="123" spans="1:48" ht="15.6" hidden="1">
       <c r="A123" s="51">
         <v>122</v>
       </c>
@@ -12700,7 +12701,7 @@
       <c r="AU123" s="1"/>
       <c r="AV123" s="1"/>
     </row>
-    <row r="124" spans="1:48" ht="15.6">
+    <row r="124" spans="1:48" ht="15.6" hidden="1">
       <c r="A124">
         <v>123</v>
       </c>
@@ -12775,7 +12776,7 @@
       <c r="AU124" s="1"/>
       <c r="AV124" s="1"/>
     </row>
-    <row r="125" spans="1:48" ht="15.6">
+    <row r="125" spans="1:48" ht="15.6" hidden="1">
       <c r="A125">
         <v>124</v>
       </c>
@@ -12850,7 +12851,7 @@
       <c r="AU125" s="1"/>
       <c r="AV125" s="1"/>
     </row>
-    <row r="126" spans="1:48" ht="15.6">
+    <row r="126" spans="1:48" ht="15.6" hidden="1">
       <c r="A126">
         <v>125</v>
       </c>
@@ -12925,7 +12926,7 @@
       <c r="AU126" s="1"/>
       <c r="AV126" s="1"/>
     </row>
-    <row r="127" spans="1:48" ht="15.6">
+    <row r="127" spans="1:48" ht="15.6" hidden="1">
       <c r="A127">
         <v>126</v>
       </c>
@@ -13000,7 +13001,7 @@
       <c r="AU127" s="1"/>
       <c r="AV127" s="1"/>
     </row>
-    <row r="128" spans="1:48" ht="15.6">
+    <row r="128" spans="1:48" ht="15.6" hidden="1">
       <c r="A128" s="51">
         <v>127</v>
       </c>
@@ -13074,7 +13075,7 @@
       <c r="AU128" s="1"/>
       <c r="AV128" s="1"/>
     </row>
-    <row r="129" spans="1:48" ht="15.6">
+    <row r="129" spans="1:48" ht="15.6" hidden="1">
       <c r="A129">
         <v>128</v>
       </c>
@@ -13148,7 +13149,7 @@
       <c r="AU129" s="1"/>
       <c r="AV129" s="1"/>
     </row>
-    <row r="130" spans="1:48" ht="15.6">
+    <row r="130" spans="1:48" ht="15.6" hidden="1">
       <c r="A130">
         <v>129</v>
       </c>
@@ -13224,7 +13225,7 @@
       <c r="AU130" s="1"/>
       <c r="AV130" s="1"/>
     </row>
-    <row r="131" spans="1:48" ht="15.6">
+    <row r="131" spans="1:48" ht="15.6" hidden="1">
       <c r="A131">
         <v>130</v>
       </c>
@@ -13305,7 +13306,7 @@
         <v>238</v>
       </c>
       <c r="C132" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D132" s="17" t="s">
         <v>75</v>
@@ -13367,7 +13368,7 @@
       <c r="AU132" s="1"/>
       <c r="AV132" s="1"/>
     </row>
-    <row r="133" spans="1:48" ht="15.6">
+    <row r="133" spans="1:48" ht="15.6" hidden="1">
       <c r="A133" s="51">
         <v>132</v>
       </c>
@@ -13439,7 +13440,7 @@
       <c r="AU133" s="1"/>
       <c r="AV133" s="1"/>
     </row>
-    <row r="134" spans="1:48" ht="15.6">
+    <row r="134" spans="1:48" ht="15.6" hidden="1">
       <c r="A134">
         <v>133</v>
       </c>
@@ -13521,7 +13522,7 @@
         <v>238</v>
       </c>
       <c r="C135" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D135" s="17" t="s">
         <v>75</v>
@@ -13587,7 +13588,7 @@
       <c r="AU135" s="1"/>
       <c r="AV135" s="1"/>
     </row>
-    <row r="136" spans="1:48" ht="15.6">
+    <row r="136" spans="1:48" ht="15.6" hidden="1">
       <c r="A136">
         <v>135</v>
       </c>
@@ -13729,7 +13730,7 @@
       <c r="AU137" s="1"/>
       <c r="AV137" s="1"/>
     </row>
-    <row r="138" spans="1:48" ht="15.6">
+    <row r="138" spans="1:48" ht="15.6" hidden="1">
       <c r="A138" s="51">
         <v>138</v>
       </c>
@@ -13803,7 +13804,7 @@
       <c r="AU138" s="1"/>
       <c r="AV138" s="1"/>
     </row>
-    <row r="139" spans="1:48" ht="15.6">
+    <row r="139" spans="1:48" ht="15.6" hidden="1">
       <c r="A139">
         <v>139</v>
       </c>
@@ -13869,7 +13870,7 @@
       <c r="AU139" s="1"/>
       <c r="AV139" s="1"/>
     </row>
-    <row r="140" spans="1:48" ht="15.6">
+    <row r="140" spans="1:48" ht="15.6" hidden="1">
       <c r="D140" s="17"/>
       <c r="E140" s="14"/>
       <c r="F140" s="14"/>
@@ -13920,7 +13921,7 @@
       <c r="AU140" s="1"/>
       <c r="AV140" s="1"/>
     </row>
-    <row r="141" spans="1:48" ht="15.6">
+    <row r="141" spans="1:48" ht="15.6" hidden="1">
       <c r="D141" s="17"/>
       <c r="E141" s="15"/>
       <c r="F141" s="14"/>
@@ -13971,7 +13972,7 @@
       <c r="AU141" s="1"/>
       <c r="AV141" s="1"/>
     </row>
-    <row r="142" spans="1:48" ht="15.6">
+    <row r="142" spans="1:48" ht="15.6" hidden="1">
       <c r="D142" s="17"/>
       <c r="E142" s="15"/>
       <c r="F142" s="14"/>
@@ -14022,7 +14023,7 @@
       <c r="AU142" s="1"/>
       <c r="AV142" s="1"/>
     </row>
-    <row r="143" spans="1:48" ht="15.6">
+    <row r="143" spans="1:48" ht="15.6" hidden="1">
       <c r="A143" s="51"/>
       <c r="B143" s="51"/>
       <c r="D143" s="17"/>
@@ -14075,7 +14076,7 @@
       <c r="AU143" s="1"/>
       <c r="AV143" s="1"/>
     </row>
-    <row r="144" spans="1:48" ht="15.6">
+    <row r="144" spans="1:48" ht="15.6" hidden="1">
       <c r="D144" s="17"/>
       <c r="E144" s="15"/>
       <c r="F144" s="14"/>
@@ -14126,7 +14127,7 @@
       <c r="AU144" s="1"/>
       <c r="AV144" s="1"/>
     </row>
-    <row r="145" spans="1:48" ht="15.6">
+    <row r="145" spans="1:48" ht="15.6" hidden="1">
       <c r="D145" s="17"/>
       <c r="E145" s="15"/>
       <c r="F145" s="14"/>
@@ -14177,7 +14178,7 @@
       <c r="AU145" s="1"/>
       <c r="AV145" s="1"/>
     </row>
-    <row r="146" spans="1:48" ht="15.6">
+    <row r="146" spans="1:48" ht="15.6" hidden="1">
       <c r="D146" s="17"/>
       <c r="E146" s="15"/>
       <c r="F146" s="14"/>
@@ -14228,7 +14229,7 @@
       <c r="AU146" s="1"/>
       <c r="AV146" s="1"/>
     </row>
-    <row r="147" spans="1:48" ht="15.6">
+    <row r="147" spans="1:48" ht="15.6" hidden="1">
       <c r="D147" s="17"/>
       <c r="E147" s="15"/>
       <c r="F147" s="14"/>
@@ -14279,7 +14280,7 @@
       <c r="AU147" s="1"/>
       <c r="AV147" s="1"/>
     </row>
-    <row r="148" spans="1:48" ht="15.6">
+    <row r="148" spans="1:48" ht="15.6" hidden="1">
       <c r="A148" s="51"/>
       <c r="B148" s="51"/>
       <c r="D148" s="17"/>
@@ -14332,7 +14333,7 @@
       <c r="AU148" s="1"/>
       <c r="AV148" s="1"/>
     </row>
-    <row r="149" spans="1:48" ht="15.6">
+    <row r="149" spans="1:48" ht="15.6" hidden="1">
       <c r="D149" s="17"/>
       <c r="E149" s="15"/>
       <c r="F149" s="15"/>
@@ -14383,7 +14384,7 @@
       <c r="AU149" s="1"/>
       <c r="AV149" s="1"/>
     </row>
-    <row r="150" spans="1:48" ht="15.6">
+    <row r="150" spans="1:48" ht="15.6" hidden="1">
       <c r="D150" s="17"/>
       <c r="E150" s="15"/>
       <c r="F150" s="15"/>
@@ -14434,7 +14435,7 @@
       <c r="AU150" s="1"/>
       <c r="AV150" s="1"/>
     </row>
-    <row r="151" spans="1:48" ht="15.6">
+    <row r="151" spans="1:48" ht="15.6" hidden="1">
       <c r="D151" s="17"/>
       <c r="E151" s="15"/>
       <c r="F151" s="15"/>
@@ -14485,7 +14486,7 @@
       <c r="AU151" s="1"/>
       <c r="AV151" s="1"/>
     </row>
-    <row r="152" spans="1:48" ht="15.6">
+    <row r="152" spans="1:48" ht="15.6" hidden="1">
       <c r="D152" s="17"/>
       <c r="E152" s="15"/>
       <c r="F152" s="15"/>
@@ -14536,7 +14537,7 @@
       <c r="AU152" s="1"/>
       <c r="AV152" s="1"/>
     </row>
-    <row r="153" spans="1:48" ht="15.6">
+    <row r="153" spans="1:48" ht="15.6" hidden="1">
       <c r="A153" s="51"/>
       <c r="B153" s="51"/>
       <c r="D153" s="17"/>
@@ -14589,7 +14590,7 @@
       <c r="AU153" s="1"/>
       <c r="AV153" s="1"/>
     </row>
-    <row r="154" spans="1:48" ht="15.6">
+    <row r="154" spans="1:48" ht="15.6" hidden="1">
       <c r="D154" s="17"/>
       <c r="E154" s="15"/>
       <c r="F154" s="15"/>
@@ -14638,7 +14639,7 @@
       <c r="AU154" s="1"/>
       <c r="AV154" s="1"/>
     </row>
-    <row r="155" spans="1:48" ht="15.6">
+    <row r="155" spans="1:48" ht="15.6" hidden="1">
       <c r="D155" s="17"/>
       <c r="E155" s="15"/>
       <c r="F155" s="15"/>
@@ -14687,7 +14688,7 @@
       <c r="AU155" s="1"/>
       <c r="AV155" s="1"/>
     </row>
-    <row r="156" spans="1:48" ht="15.6">
+    <row r="156" spans="1:48" ht="15.6" hidden="1">
       <c r="D156" s="17"/>
       <c r="E156" s="15"/>
       <c r="F156" s="15"/>
@@ -14736,7 +14737,7 @@
       <c r="AU156" s="1"/>
       <c r="AV156" s="1"/>
     </row>
-    <row r="157" spans="1:48" ht="15.6">
+    <row r="157" spans="1:48" ht="15.6" hidden="1">
       <c r="D157" s="17"/>
       <c r="E157" s="15"/>
       <c r="F157" s="15"/>
@@ -14785,7 +14786,7 @@
       <c r="AU157" s="1"/>
       <c r="AV157" s="1"/>
     </row>
-    <row r="158" spans="1:48" ht="15.6">
+    <row r="158" spans="1:48" ht="15.6" hidden="1">
       <c r="A158" s="51"/>
       <c r="B158" s="51"/>
       <c r="D158" s="17"/>
@@ -14836,7 +14837,7 @@
       <c r="AU158" s="1"/>
       <c r="AV158" s="1"/>
     </row>
-    <row r="159" spans="1:48" ht="15.6">
+    <row r="159" spans="1:48" ht="15.6" hidden="1">
       <c r="D159" s="17"/>
       <c r="E159" s="15"/>
       <c r="F159" s="15"/>
@@ -14885,7 +14886,7 @@
       <c r="AU159" s="1"/>
       <c r="AV159" s="1"/>
     </row>
-    <row r="160" spans="1:48" ht="15.6">
+    <row r="160" spans="1:48" ht="15.6" hidden="1">
       <c r="D160" s="17"/>
       <c r="E160" s="15"/>
       <c r="F160" s="15"/>
@@ -14934,7 +14935,7 @@
       <c r="AU160" s="1"/>
       <c r="AV160" s="1"/>
     </row>
-    <row r="161" spans="1:48" ht="15.6">
+    <row r="161" spans="1:48" ht="15.6" hidden="1">
       <c r="D161" s="17"/>
       <c r="E161" s="15"/>
       <c r="F161" s="15"/>
@@ -14983,7 +14984,7 @@
       <c r="AU161" s="1"/>
       <c r="AV161" s="1"/>
     </row>
-    <row r="162" spans="1:48" ht="15.6">
+    <row r="162" spans="1:48" ht="15.6" hidden="1">
       <c r="D162" s="17"/>
       <c r="E162" s="15"/>
       <c r="F162" s="15"/>
@@ -15032,7 +15033,7 @@
       <c r="AU162" s="1"/>
       <c r="AV162" s="1"/>
     </row>
-    <row r="163" spans="1:48" ht="15.6">
+    <row r="163" spans="1:48" ht="15.6" hidden="1">
       <c r="A163" s="51"/>
       <c r="B163" s="51"/>
       <c r="D163" s="17"/>
@@ -15083,7 +15084,7 @@
       <c r="AU163" s="1"/>
       <c r="AV163" s="1"/>
     </row>
-    <row r="164" spans="1:48" ht="15.6">
+    <row r="164" spans="1:48" ht="15.6" hidden="1">
       <c r="D164" s="17"/>
       <c r="E164" s="15"/>
       <c r="F164" s="15"/>
@@ -15132,7 +15133,7 @@
       <c r="AU164" s="1"/>
       <c r="AV164" s="1"/>
     </row>
-    <row r="165" spans="1:48">
+    <row r="165" spans="1:48" hidden="1">
       <c r="D165" s="17"/>
       <c r="E165" s="15"/>
       <c r="F165" s="15"/>
@@ -15181,7 +15182,7 @@
       <c r="AU165" s="1"/>
       <c r="AV165" s="1"/>
     </row>
-    <row r="166" spans="1:48">
+    <row r="166" spans="1:48" hidden="1">
       <c r="D166" s="17"/>
       <c r="E166" s="15"/>
       <c r="F166" s="15"/>
@@ -15230,7 +15231,7 @@
       <c r="AU166" s="1"/>
       <c r="AV166" s="1"/>
     </row>
-    <row r="167" spans="1:48">
+    <row r="167" spans="1:48" hidden="1">
       <c r="D167" s="17"/>
       <c r="E167" s="15"/>
       <c r="F167" s="15"/>
@@ -15279,7 +15280,7 @@
       <c r="AU167" s="1"/>
       <c r="AV167" s="1"/>
     </row>
-    <row r="168" spans="1:48">
+    <row r="168" spans="1:48" hidden="1">
       <c r="A168" s="51"/>
       <c r="B168" s="51"/>
       <c r="D168" s="17"/>
@@ -15330,7 +15331,7 @@
       <c r="AU168" s="1"/>
       <c r="AV168" s="1"/>
     </row>
-    <row r="169" spans="1:48">
+    <row r="169" spans="1:48" hidden="1">
       <c r="D169" s="17"/>
       <c r="E169" s="15"/>
       <c r="F169" s="15"/>
@@ -15379,7 +15380,7 @@
       <c r="AU169" s="1"/>
       <c r="AV169" s="1"/>
     </row>
-    <row r="170" spans="1:48">
+    <row r="170" spans="1:48" hidden="1">
       <c r="D170" s="17"/>
       <c r="E170" s="15"/>
       <c r="F170" s="15"/>
@@ -15428,7 +15429,7 @@
       <c r="AU170" s="1"/>
       <c r="AV170" s="1"/>
     </row>
-    <row r="171" spans="1:48">
+    <row r="171" spans="1:48" hidden="1">
       <c r="D171" s="17"/>
       <c r="E171" s="15"/>
       <c r="F171" s="15"/>
@@ -15477,7 +15478,7 @@
       <c r="AU171" s="1"/>
       <c r="AV171" s="1"/>
     </row>
-    <row r="172" spans="1:48">
+    <row r="172" spans="1:48" hidden="1">
       <c r="D172" s="17"/>
       <c r="E172" s="15"/>
       <c r="F172" s="15"/>
@@ -15526,7 +15527,7 @@
       <c r="AU172" s="1"/>
       <c r="AV172" s="1"/>
     </row>
-    <row r="173" spans="1:48">
+    <row r="173" spans="1:48" hidden="1">
       <c r="A173" s="51"/>
       <c r="B173" s="51"/>
       <c r="D173" s="17"/>
@@ -15577,7 +15578,7 @@
       <c r="AU173" s="1"/>
       <c r="AV173" s="1"/>
     </row>
-    <row r="174" spans="1:48">
+    <row r="174" spans="1:48" hidden="1">
       <c r="D174" s="17"/>
       <c r="E174" s="15"/>
       <c r="F174" s="15"/>
@@ -15626,7 +15627,7 @@
       <c r="AU174" s="1"/>
       <c r="AV174" s="1"/>
     </row>
-    <row r="175" spans="1:48">
+    <row r="175" spans="1:48" hidden="1">
       <c r="D175" s="17"/>
       <c r="E175" s="15"/>
       <c r="F175" s="15"/>
@@ -15675,7 +15676,7 @@
       <c r="AU175" s="1"/>
       <c r="AV175" s="1"/>
     </row>
-    <row r="176" spans="1:48">
+    <row r="176" spans="1:48" hidden="1">
       <c r="D176" s="17"/>
       <c r="E176" s="15"/>
       <c r="F176" s="15"/>
@@ -15724,7 +15725,7 @@
       <c r="AU176" s="1"/>
       <c r="AV176" s="1"/>
     </row>
-    <row r="177" spans="1:48">
+    <row r="177" spans="1:48" hidden="1">
       <c r="D177" s="17"/>
       <c r="E177" s="15"/>
       <c r="F177" s="15"/>
@@ -15773,7 +15774,7 @@
       <c r="AU177" s="1"/>
       <c r="AV177" s="1"/>
     </row>
-    <row r="178" spans="1:48">
+    <row r="178" spans="1:48" hidden="1">
       <c r="A178" s="51"/>
       <c r="B178" s="51"/>
       <c r="D178" s="17"/>
@@ -15824,7 +15825,7 @@
       <c r="AU178" s="1"/>
       <c r="AV178" s="1"/>
     </row>
-    <row r="179" spans="1:48">
+    <row r="179" spans="1:48" hidden="1">
       <c r="D179" s="17"/>
       <c r="E179" s="15"/>
       <c r="F179" s="15"/>
@@ -15873,7 +15874,7 @@
       <c r="AU179" s="1"/>
       <c r="AV179" s="1"/>
     </row>
-    <row r="180" spans="1:48">
+    <row r="180" spans="1:48" hidden="1">
       <c r="D180" s="17"/>
       <c r="E180" s="15"/>
       <c r="F180" s="15"/>
@@ -15922,7 +15923,7 @@
       <c r="AU180" s="1"/>
       <c r="AV180" s="1"/>
     </row>
-    <row r="181" spans="1:48">
+    <row r="181" spans="1:48" hidden="1">
       <c r="D181" s="17"/>
       <c r="E181" s="15"/>
       <c r="F181" s="15"/>
@@ -15971,7 +15972,7 @@
       <c r="AU181" s="1"/>
       <c r="AV181" s="1"/>
     </row>
-    <row r="182" spans="1:48">
+    <row r="182" spans="1:48" hidden="1">
       <c r="D182" s="17"/>
       <c r="E182" s="15"/>
       <c r="F182" s="15"/>
@@ -16020,7 +16021,7 @@
       <c r="AU182" s="1"/>
       <c r="AV182" s="1"/>
     </row>
-    <row r="183" spans="1:48">
+    <row r="183" spans="1:48" hidden="1">
       <c r="A183" s="51"/>
       <c r="B183" s="51"/>
       <c r="D183" s="17"/>
@@ -16071,7 +16072,7 @@
       <c r="AU183" s="1"/>
       <c r="AV183" s="1"/>
     </row>
-    <row r="184" spans="1:48">
+    <row r="184" spans="1:48" hidden="1">
       <c r="D184" s="17"/>
       <c r="E184" s="15"/>
       <c r="F184" s="15"/>
@@ -16120,7 +16121,7 @@
       <c r="AU184" s="1"/>
       <c r="AV184" s="1"/>
     </row>
-    <row r="185" spans="1:48">
+    <row r="185" spans="1:48" hidden="1">
       <c r="D185" s="17"/>
       <c r="E185" s="15"/>
       <c r="F185" s="15"/>
@@ -16169,7 +16170,7 @@
       <c r="AU185" s="1"/>
       <c r="AV185" s="1"/>
     </row>
-    <row r="186" spans="1:48">
+    <row r="186" spans="1:48" hidden="1">
       <c r="D186" s="17"/>
       <c r="E186" s="15"/>
       <c r="F186" s="15"/>
@@ -16218,7 +16219,7 @@
       <c r="AU186" s="1"/>
       <c r="AV186" s="1"/>
     </row>
-    <row r="187" spans="1:48">
+    <row r="187" spans="1:48" hidden="1">
       <c r="D187" s="17"/>
       <c r="E187" s="15"/>
       <c r="F187" s="15"/>
@@ -16267,7 +16268,7 @@
       <c r="AU187" s="1"/>
       <c r="AV187" s="1"/>
     </row>
-    <row r="188" spans="1:48">
+    <row r="188" spans="1:48" hidden="1">
       <c r="A188" s="51"/>
       <c r="B188" s="51"/>
       <c r="D188" s="17"/>
@@ -16318,7 +16319,7 @@
       <c r="AU188" s="1"/>
       <c r="AV188" s="1"/>
     </row>
-    <row r="189" spans="1:48">
+    <row r="189" spans="1:48" hidden="1">
       <c r="D189" s="17"/>
       <c r="E189" s="15"/>
       <c r="F189" s="15"/>
@@ -16367,7 +16368,7 @@
       <c r="AU189" s="1"/>
       <c r="AV189" s="1"/>
     </row>
-    <row r="190" spans="1:48">
+    <row r="190" spans="1:48" hidden="1">
       <c r="D190" s="17"/>
       <c r="E190" s="15"/>
       <c r="F190" s="15"/>
@@ -16416,7 +16417,7 @@
       <c r="AU190" s="1"/>
       <c r="AV190" s="1"/>
     </row>
-    <row r="191" spans="1:48">
+    <row r="191" spans="1:48" hidden="1">
       <c r="D191" s="17"/>
       <c r="E191" s="15"/>
       <c r="F191" s="15"/>
@@ -16465,7 +16466,7 @@
       <c r="AU191" s="1"/>
       <c r="AV191" s="1"/>
     </row>
-    <row r="192" spans="1:48">
+    <row r="192" spans="1:48" hidden="1">
       <c r="D192" s="17"/>
       <c r="E192" s="15"/>
       <c r="F192" s="15"/>
@@ -16514,7 +16515,7 @@
       <c r="AU192" s="1"/>
       <c r="AV192" s="1"/>
     </row>
-    <row r="193" spans="1:48">
+    <row r="193" spans="1:48" hidden="1">
       <c r="A193" s="51"/>
       <c r="B193" s="51"/>
       <c r="D193" s="17"/>
@@ -16565,7 +16566,7 @@
       <c r="AU193" s="1"/>
       <c r="AV193" s="1"/>
     </row>
-    <row r="194" spans="1:48">
+    <row r="194" spans="1:48" hidden="1">
       <c r="D194" s="17"/>
       <c r="E194" s="15"/>
       <c r="F194" s="15"/>
@@ -16614,7 +16615,7 @@
       <c r="AU194" s="1"/>
       <c r="AV194" s="1"/>
     </row>
-    <row r="195" spans="1:48">
+    <row r="195" spans="1:48" hidden="1">
       <c r="D195" s="17"/>
       <c r="E195" s="15"/>
       <c r="F195" s="15"/>
@@ -16663,7 +16664,7 @@
       <c r="AU195" s="1"/>
       <c r="AV195" s="1"/>
     </row>
-    <row r="196" spans="1:48">
+    <row r="196" spans="1:48" hidden="1">
       <c r="D196" s="17"/>
       <c r="E196" s="15"/>
       <c r="F196" s="15"/>
@@ -16712,7 +16713,7 @@
       <c r="AU196" s="1"/>
       <c r="AV196" s="1"/>
     </row>
-    <row r="197" spans="1:48">
+    <row r="197" spans="1:48" hidden="1">
       <c r="D197" s="17"/>
       <c r="E197" s="15"/>
       <c r="F197" s="15"/>
@@ -16761,7 +16762,7 @@
       <c r="AU197" s="1"/>
       <c r="AV197" s="1"/>
     </row>
-    <row r="198" spans="1:48">
+    <row r="198" spans="1:48" hidden="1">
       <c r="A198" s="51"/>
       <c r="B198" s="51"/>
       <c r="D198" s="17"/>
@@ -16812,7 +16813,7 @@
       <c r="AU198" s="1"/>
       <c r="AV198" s="1"/>
     </row>
-    <row r="199" spans="1:48">
+    <row r="199" spans="1:48" hidden="1">
       <c r="D199" s="17"/>
       <c r="E199" s="15"/>
       <c r="F199" s="15"/>
@@ -16861,7 +16862,7 @@
       <c r="AU199" s="1"/>
       <c r="AV199" s="1"/>
     </row>
-    <row r="200" spans="1:48">
+    <row r="200" spans="1:48" hidden="1">
       <c r="D200" s="17"/>
       <c r="E200" s="15"/>
       <c r="F200" s="15"/>
@@ -16910,7 +16911,7 @@
       <c r="AU200" s="1"/>
       <c r="AV200" s="1"/>
     </row>
-    <row r="201" spans="1:48">
+    <row r="201" spans="1:48" hidden="1">
       <c r="D201" s="17"/>
       <c r="E201" s="15"/>
       <c r="F201" s="15"/>
@@ -16959,7 +16960,7 @@
       <c r="AU201" s="1"/>
       <c r="AV201" s="1"/>
     </row>
-    <row r="202" spans="1:48">
+    <row r="202" spans="1:48" hidden="1">
       <c r="D202" s="17"/>
       <c r="E202" s="15"/>
       <c r="F202" s="15"/>
@@ -17008,7 +17009,7 @@
       <c r="AU202" s="1"/>
       <c r="AV202" s="1"/>
     </row>
-    <row r="203" spans="1:48">
+    <row r="203" spans="1:48" hidden="1">
       <c r="A203" s="51"/>
       <c r="B203" s="51"/>
       <c r="D203" s="17"/>
@@ -17059,7 +17060,7 @@
       <c r="AU203" s="1"/>
       <c r="AV203" s="1"/>
     </row>
-    <row r="204" spans="1:48">
+    <row r="204" spans="1:48" hidden="1">
       <c r="D204" s="17"/>
       <c r="E204" s="15"/>
       <c r="F204" s="15"/>
@@ -17108,7 +17109,7 @@
       <c r="AU204" s="1"/>
       <c r="AV204" s="1"/>
     </row>
-    <row r="205" spans="1:48">
+    <row r="205" spans="1:48" hidden="1">
       <c r="D205" s="17"/>
       <c r="E205" s="15"/>
       <c r="F205" s="15"/>
@@ -17157,7 +17158,7 @@
       <c r="AU205" s="1"/>
       <c r="AV205" s="1"/>
     </row>
-    <row r="206" spans="1:48">
+    <row r="206" spans="1:48" hidden="1">
       <c r="D206" s="17"/>
       <c r="E206" s="15"/>
       <c r="F206" s="15"/>
@@ -17206,7 +17207,7 @@
       <c r="AU206" s="1"/>
       <c r="AV206" s="1"/>
     </row>
-    <row r="207" spans="1:48">
+    <row r="207" spans="1:48" hidden="1">
       <c r="D207" s="17"/>
       <c r="E207" s="15"/>
       <c r="F207" s="15"/>
@@ -17255,7 +17256,7 @@
       <c r="AU207" s="1"/>
       <c r="AV207" s="1"/>
     </row>
-    <row r="208" spans="1:48">
+    <row r="208" spans="1:48" hidden="1">
       <c r="A208" s="51"/>
       <c r="B208" s="51"/>
       <c r="D208" s="17"/>
@@ -17306,7 +17307,7 @@
       <c r="AU208" s="1"/>
       <c r="AV208" s="1"/>
     </row>
-    <row r="209" spans="1:48">
+    <row r="209" spans="1:48" hidden="1">
       <c r="D209" s="17"/>
       <c r="E209" s="15"/>
       <c r="F209" s="15"/>
@@ -17355,7 +17356,7 @@
       <c r="AU209" s="1"/>
       <c r="AV209" s="1"/>
     </row>
-    <row r="210" spans="1:48">
+    <row r="210" spans="1:48" hidden="1">
       <c r="D210" s="17"/>
       <c r="E210" s="15"/>
       <c r="F210" s="15"/>
@@ -17404,7 +17405,7 @@
       <c r="AU210" s="1"/>
       <c r="AV210" s="1"/>
     </row>
-    <row r="211" spans="1:48">
+    <row r="211" spans="1:48" hidden="1">
       <c r="D211" s="17"/>
       <c r="E211" s="15"/>
       <c r="F211" s="15"/>
@@ -17453,7 +17454,7 @@
       <c r="AU211" s="1"/>
       <c r="AV211" s="1"/>
     </row>
-    <row r="212" spans="1:48">
+    <row r="212" spans="1:48" hidden="1">
       <c r="D212" s="17"/>
       <c r="E212" s="15"/>
       <c r="F212" s="15"/>
@@ -17502,7 +17503,7 @@
       <c r="AU212" s="1"/>
       <c r="AV212" s="1"/>
     </row>
-    <row r="213" spans="1:48">
+    <row r="213" spans="1:48" hidden="1">
       <c r="A213" s="51"/>
       <c r="B213" s="51"/>
       <c r="D213" s="17"/>
@@ -17553,7 +17554,7 @@
       <c r="AU213" s="1"/>
       <c r="AV213" s="1"/>
     </row>
-    <row r="214" spans="1:48">
+    <row r="214" spans="1:48" hidden="1">
       <c r="D214" s="17"/>
       <c r="E214" s="15"/>
       <c r="F214" s="15"/>
@@ -17602,7 +17603,7 @@
       <c r="AU214" s="1"/>
       <c r="AV214" s="1"/>
     </row>
-    <row r="215" spans="1:48">
+    <row r="215" spans="1:48" hidden="1">
       <c r="D215" s="17"/>
       <c r="E215" s="15"/>
       <c r="F215" s="15"/>
@@ -17651,7 +17652,7 @@
       <c r="AU215" s="1"/>
       <c r="AV215" s="1"/>
     </row>
-    <row r="216" spans="1:48">
+    <row r="216" spans="1:48" hidden="1">
       <c r="D216" s="17"/>
       <c r="E216" s="15"/>
       <c r="F216" s="15"/>
@@ -17700,7 +17701,7 @@
       <c r="AU216" s="1"/>
       <c r="AV216" s="1"/>
     </row>
-    <row r="217" spans="1:48">
+    <row r="217" spans="1:48" hidden="1">
       <c r="D217" s="17"/>
       <c r="E217" s="15"/>
       <c r="F217" s="15"/>
@@ -17727,7 +17728,7 @@
       <c r="Y217" s="2"/>
       <c r="Z217" s="2"/>
     </row>
-    <row r="218" spans="1:48">
+    <row r="218" spans="1:48" hidden="1">
       <c r="A218" s="51"/>
       <c r="B218" s="51"/>
       <c r="D218" s="17"/>
@@ -17756,7 +17757,7 @@
       <c r="Y218" s="2"/>
       <c r="Z218" s="2"/>
     </row>
-    <row r="219" spans="1:48">
+    <row r="219" spans="1:48" hidden="1">
       <c r="D219" s="17"/>
       <c r="E219" s="15"/>
       <c r="F219" s="15"/>
@@ -17783,7 +17784,7 @@
       <c r="Y219" s="2"/>
       <c r="Z219" s="2"/>
     </row>
-    <row r="220" spans="1:48">
+    <row r="220" spans="1:48" hidden="1">
       <c r="D220" s="17"/>
       <c r="E220" s="15"/>
       <c r="F220" s="15"/>
@@ -17810,7 +17811,7 @@
       <c r="Y220" s="2"/>
       <c r="Z220" s="2"/>
     </row>
-    <row r="221" spans="1:48">
+    <row r="221" spans="1:48" hidden="1">
       <c r="D221" s="17"/>
       <c r="E221" s="15"/>
       <c r="F221" s="15"/>
@@ -17837,7 +17838,7 @@
       <c r="Y221" s="2"/>
       <c r="Z221" s="2"/>
     </row>
-    <row r="222" spans="1:48">
+    <row r="222" spans="1:48" hidden="1">
       <c r="D222" s="17"/>
       <c r="E222" s="15"/>
       <c r="F222" s="15"/>
@@ -17864,7 +17865,7 @@
       <c r="Y222" s="2"/>
       <c r="Z222" s="2"/>
     </row>
-    <row r="223" spans="1:48">
+    <row r="223" spans="1:48" hidden="1">
       <c r="A223" s="51"/>
       <c r="B223" s="51"/>
       <c r="D223" s="17"/>
@@ -17893,7 +17894,7 @@
       <c r="Y223" s="2"/>
       <c r="Z223" s="2"/>
     </row>
-    <row r="224" spans="1:48">
+    <row r="224" spans="1:48" hidden="1">
       <c r="D224" s="17"/>
       <c r="E224" s="15"/>
       <c r="F224" s="15"/>
@@ -17920,7 +17921,7 @@
       <c r="Y224" s="2"/>
       <c r="Z224" s="2"/>
     </row>
-    <row r="225" spans="1:26">
+    <row r="225" spans="1:26" hidden="1">
       <c r="D225" s="17"/>
       <c r="E225" s="15"/>
       <c r="F225" s="15"/>
@@ -17947,7 +17948,7 @@
       <c r="Y225" s="2"/>
       <c r="Z225" s="2"/>
     </row>
-    <row r="226" spans="1:26">
+    <row r="226" spans="1:26" hidden="1">
       <c r="D226" s="17"/>
       <c r="E226" s="15"/>
       <c r="F226" s="15"/>
@@ -17974,7 +17975,7 @@
       <c r="Y226" s="2"/>
       <c r="Z226" s="2"/>
     </row>
-    <row r="227" spans="1:26">
+    <row r="227" spans="1:26" hidden="1">
       <c r="D227" s="17"/>
       <c r="E227" s="15"/>
       <c r="F227" s="15"/>
@@ -18001,7 +18002,7 @@
       <c r="Y227" s="2"/>
       <c r="Z227" s="2"/>
     </row>
-    <row r="228" spans="1:26">
+    <row r="228" spans="1:26" hidden="1">
       <c r="A228" s="51"/>
       <c r="B228" s="51"/>
       <c r="D228" s="17"/>
@@ -18030,7 +18031,7 @@
       <c r="Y228" s="2"/>
       <c r="Z228" s="2"/>
     </row>
-    <row r="229" spans="1:26">
+    <row r="229" spans="1:26" hidden="1">
       <c r="D229" s="17"/>
       <c r="E229" s="15"/>
       <c r="F229" s="15"/>
@@ -18057,7 +18058,7 @@
       <c r="Y229" s="2"/>
       <c r="Z229" s="2"/>
     </row>
-    <row r="230" spans="1:26">
+    <row r="230" spans="1:26" hidden="1">
       <c r="D230" s="17"/>
       <c r="E230" s="15"/>
       <c r="F230" s="15"/>
@@ -18084,7 +18085,7 @@
       <c r="Y230" s="2"/>
       <c r="Z230" s="2"/>
     </row>
-    <row r="231" spans="1:26">
+    <row r="231" spans="1:26" hidden="1">
       <c r="D231" s="17"/>
       <c r="E231" s="15"/>
       <c r="F231" s="15"/>
@@ -18111,7 +18112,7 @@
       <c r="Y231" s="2"/>
       <c r="Z231" s="2"/>
     </row>
-    <row r="232" spans="1:26">
+    <row r="232" spans="1:26" hidden="1">
       <c r="D232" s="17"/>
       <c r="E232" s="15"/>
       <c r="F232" s="15"/>
@@ -18138,7 +18139,7 @@
       <c r="Y232" s="2"/>
       <c r="Z232" s="2"/>
     </row>
-    <row r="233" spans="1:26">
+    <row r="233" spans="1:26" hidden="1">
       <c r="A233" s="51"/>
       <c r="B233" s="51"/>
       <c r="D233" s="17"/>
@@ -18167,7 +18168,7 @@
       <c r="Y233" s="2"/>
       <c r="Z233" s="2"/>
     </row>
-    <row r="234" spans="1:26">
+    <row r="234" spans="1:26" hidden="1">
       <c r="D234" s="17"/>
       <c r="E234" s="15"/>
       <c r="F234" s="15"/>
@@ -18194,7 +18195,7 @@
       <c r="Y234" s="2"/>
       <c r="Z234" s="2"/>
     </row>
-    <row r="235" spans="1:26">
+    <row r="235" spans="1:26" hidden="1">
       <c r="D235" s="17"/>
       <c r="E235" s="15"/>
       <c r="F235" s="15"/>
@@ -18221,7 +18222,7 @@
       <c r="Y235" s="2"/>
       <c r="Z235" s="2"/>
     </row>
-    <row r="236" spans="1:26">
+    <row r="236" spans="1:26" hidden="1">
       <c r="D236" s="17"/>
       <c r="E236" s="15"/>
       <c r="F236" s="15"/>
@@ -18248,7 +18249,7 @@
       <c r="Y236" s="2"/>
       <c r="Z236" s="2"/>
     </row>
-    <row r="237" spans="1:26">
+    <row r="237" spans="1:26" hidden="1">
       <c r="D237" s="17"/>
       <c r="E237" s="15"/>
       <c r="F237" s="15"/>
@@ -18275,7 +18276,7 @@
       <c r="Y237" s="2"/>
       <c r="Z237" s="2"/>
     </row>
-    <row r="238" spans="1:26">
+    <row r="238" spans="1:26" hidden="1">
       <c r="A238" s="51"/>
       <c r="B238" s="51"/>
       <c r="D238" s="17"/>
@@ -18304,7 +18305,7 @@
       <c r="Y238" s="2"/>
       <c r="Z238" s="2"/>
     </row>
-    <row r="239" spans="1:26">
+    <row r="239" spans="1:26" hidden="1">
       <c r="D239" s="17"/>
       <c r="E239" s="15"/>
       <c r="F239" s="15"/>
@@ -18331,7 +18332,7 @@
       <c r="Y239" s="2"/>
       <c r="Z239" s="2"/>
     </row>
-    <row r="240" spans="1:26">
+    <row r="240" spans="1:26" hidden="1">
       <c r="D240" s="17"/>
       <c r="E240" s="15"/>
       <c r="F240" s="15"/>
@@ -18358,7 +18359,7 @@
       <c r="Y240" s="2"/>
       <c r="Z240" s="2"/>
     </row>
-    <row r="241" spans="1:26">
+    <row r="241" spans="1:26" hidden="1">
       <c r="D241" s="17"/>
       <c r="E241" s="15"/>
       <c r="F241" s="15"/>
@@ -18385,7 +18386,7 @@
       <c r="Y241" s="2"/>
       <c r="Z241" s="2"/>
     </row>
-    <row r="242" spans="1:26">
+    <row r="242" spans="1:26" hidden="1">
       <c r="D242" s="17"/>
       <c r="E242" s="15"/>
       <c r="F242" s="15"/>
@@ -18412,7 +18413,7 @@
       <c r="Y242" s="2"/>
       <c r="Z242" s="2"/>
     </row>
-    <row r="243" spans="1:26">
+    <row r="243" spans="1:26" hidden="1">
       <c r="A243" s="51"/>
       <c r="B243" s="51"/>
       <c r="D243" s="17"/>
@@ -18441,7 +18442,7 @@
       <c r="Y243" s="2"/>
       <c r="Z243" s="2"/>
     </row>
-    <row r="244" spans="1:26">
+    <row r="244" spans="1:26" hidden="1">
       <c r="D244" s="17"/>
       <c r="E244" s="15"/>
       <c r="F244" s="15"/>
@@ -18468,7 +18469,7 @@
       <c r="Y244" s="2"/>
       <c r="Z244" s="2"/>
     </row>
-    <row r="245" spans="1:26">
+    <row r="245" spans="1:26" hidden="1">
       <c r="D245" s="17"/>
       <c r="E245" s="15"/>
       <c r="F245" s="15"/>
@@ -18495,7 +18496,7 @@
       <c r="Y245" s="2"/>
       <c r="Z245" s="2"/>
     </row>
-    <row r="246" spans="1:26">
+    <row r="246" spans="1:26" hidden="1">
       <c r="D246" s="17"/>
       <c r="E246" s="15"/>
       <c r="F246" s="15"/>
@@ -18522,7 +18523,7 @@
       <c r="Y246" s="2"/>
       <c r="Z246" s="2"/>
     </row>
-    <row r="247" spans="1:26">
+    <row r="247" spans="1:26" hidden="1">
       <c r="D247" s="17"/>
       <c r="E247" s="15"/>
       <c r="F247" s="15"/>
@@ -18549,7 +18550,7 @@
       <c r="Y247" s="2"/>
       <c r="Z247" s="2"/>
     </row>
-    <row r="248" spans="1:26">
+    <row r="248" spans="1:26" hidden="1">
       <c r="A248" s="51"/>
       <c r="B248" s="51"/>
       <c r="D248" s="17"/>
@@ -18578,7 +18579,7 @@
       <c r="Y248" s="2"/>
       <c r="Z248" s="2"/>
     </row>
-    <row r="249" spans="1:26">
+    <row r="249" spans="1:26" hidden="1">
       <c r="D249" s="17"/>
       <c r="E249" s="15"/>
       <c r="F249" s="15"/>
@@ -18605,7 +18606,7 @@
       <c r="Y249" s="2"/>
       <c r="Z249" s="2"/>
     </row>
-    <row r="250" spans="1:26">
+    <row r="250" spans="1:26" hidden="1">
       <c r="D250" s="17"/>
       <c r="E250" s="15"/>
       <c r="F250" s="15"/>
@@ -18632,7 +18633,7 @@
       <c r="Y250" s="2"/>
       <c r="Z250" s="2"/>
     </row>
-    <row r="251" spans="1:26">
+    <row r="251" spans="1:26" hidden="1">
       <c r="D251" s="17"/>
       <c r="E251" s="15"/>
       <c r="F251" s="15"/>
@@ -18659,7 +18660,7 @@
       <c r="Y251" s="2"/>
       <c r="Z251" s="2"/>
     </row>
-    <row r="252" spans="1:26">
+    <row r="252" spans="1:26" hidden="1">
       <c r="D252" s="17"/>
       <c r="E252" s="15"/>
       <c r="F252" s="15"/>
@@ -18686,7 +18687,7 @@
       <c r="Y252" s="2"/>
       <c r="Z252" s="2"/>
     </row>
-    <row r="253" spans="1:26">
+    <row r="253" spans="1:26" hidden="1">
       <c r="A253" s="51"/>
       <c r="B253" s="51"/>
       <c r="D253" s="17"/>
@@ -18715,7 +18716,7 @@
       <c r="Y253" s="2"/>
       <c r="Z253" s="2"/>
     </row>
-    <row r="254" spans="1:26">
+    <row r="254" spans="1:26" hidden="1">
       <c r="D254" s="17"/>
       <c r="E254" s="15"/>
       <c r="F254" s="15"/>
@@ -18742,7 +18743,7 @@
       <c r="Y254" s="2"/>
       <c r="Z254" s="2"/>
     </row>
-    <row r="255" spans="1:26">
+    <row r="255" spans="1:26" hidden="1">
       <c r="D255" s="17"/>
       <c r="E255" s="15"/>
       <c r="F255" s="15"/>
@@ -18769,7 +18770,7 @@
       <c r="Y255" s="2"/>
       <c r="Z255" s="2"/>
     </row>
-    <row r="256" spans="1:26">
+    <row r="256" spans="1:26" hidden="1">
       <c r="D256" s="17"/>
       <c r="E256" s="15"/>
       <c r="F256" s="15"/>
@@ -18796,7 +18797,7 @@
       <c r="Y256" s="2"/>
       <c r="Z256" s="2"/>
     </row>
-    <row r="257" spans="1:26">
+    <row r="257" spans="1:26" hidden="1">
       <c r="D257" s="17"/>
       <c r="E257" s="15"/>
       <c r="F257" s="15"/>
@@ -18823,7 +18824,7 @@
       <c r="Y257" s="2"/>
       <c r="Z257" s="2"/>
     </row>
-    <row r="258" spans="1:26">
+    <row r="258" spans="1:26" hidden="1">
       <c r="A258" s="51"/>
       <c r="B258" s="51"/>
       <c r="D258" s="17"/>
@@ -18852,7 +18853,7 @@
       <c r="Y258" s="2"/>
       <c r="Z258" s="2"/>
     </row>
-    <row r="259" spans="1:26">
+    <row r="259" spans="1:26" hidden="1">
       <c r="D259" s="17"/>
       <c r="E259" s="15"/>
       <c r="F259" s="15"/>
@@ -18879,7 +18880,7 @@
       <c r="Y259" s="2"/>
       <c r="Z259" s="2"/>
     </row>
-    <row r="260" spans="1:26">
+    <row r="260" spans="1:26" hidden="1">
       <c r="D260" s="17"/>
       <c r="E260" s="15"/>
       <c r="F260" s="15"/>
@@ -18906,7 +18907,7 @@
       <c r="Y260" s="2"/>
       <c r="Z260" s="2"/>
     </row>
-    <row r="261" spans="1:26">
+    <row r="261" spans="1:26" hidden="1">
       <c r="D261" s="17"/>
       <c r="E261" s="15"/>
       <c r="F261" s="15"/>
@@ -18933,7 +18934,7 @@
       <c r="Y261" s="2"/>
       <c r="Z261" s="2"/>
     </row>
-    <row r="262" spans="1:26">
+    <row r="262" spans="1:26" hidden="1">
       <c r="D262" s="17"/>
       <c r="E262" s="15"/>
       <c r="F262" s="15"/>
@@ -18960,7 +18961,7 @@
       <c r="Y262" s="2"/>
       <c r="Z262" s="2"/>
     </row>
-    <row r="263" spans="1:26">
+    <row r="263" spans="1:26" hidden="1">
       <c r="A263" s="51"/>
       <c r="B263" s="51"/>
       <c r="D263" s="17"/>
@@ -18989,7 +18990,7 @@
       <c r="Y263" s="2"/>
       <c r="Z263" s="2"/>
     </row>
-    <row r="264" spans="1:26">
+    <row r="264" spans="1:26" hidden="1">
       <c r="D264" s="17"/>
       <c r="E264" s="15"/>
       <c r="F264" s="15"/>
@@ -19016,7 +19017,7 @@
       <c r="Y264" s="2"/>
       <c r="Z264" s="2"/>
     </row>
-    <row r="265" spans="1:26">
+    <row r="265" spans="1:26" hidden="1">
       <c r="D265" s="17"/>
       <c r="E265" s="15"/>
       <c r="F265" s="15"/>
@@ -19043,7 +19044,7 @@
       <c r="Y265" s="2"/>
       <c r="Z265" s="2"/>
     </row>
-    <row r="266" spans="1:26">
+    <row r="266" spans="1:26" hidden="1">
       <c r="D266" s="17"/>
       <c r="E266" s="15"/>
       <c r="F266" s="15"/>
@@ -19070,7 +19071,7 @@
       <c r="Y266" s="2"/>
       <c r="Z266" s="2"/>
     </row>
-    <row r="267" spans="1:26">
+    <row r="267" spans="1:26" hidden="1">
       <c r="D267" s="17"/>
       <c r="E267" s="15"/>
       <c r="F267" s="15"/>
@@ -19097,7 +19098,7 @@
       <c r="Y267" s="2"/>
       <c r="Z267" s="2"/>
     </row>
-    <row r="268" spans="1:26">
+    <row r="268" spans="1:26" hidden="1">
       <c r="A268" s="51"/>
       <c r="B268" s="51"/>
       <c r="D268" s="17"/>
@@ -19126,7 +19127,7 @@
       <c r="Y268" s="2"/>
       <c r="Z268" s="2"/>
     </row>
-    <row r="269" spans="1:26">
+    <row r="269" spans="1:26" hidden="1">
       <c r="D269" s="17"/>
       <c r="E269" s="15"/>
       <c r="F269" s="15"/>
@@ -19153,7 +19154,7 @@
       <c r="Y269" s="2"/>
       <c r="Z269" s="2"/>
     </row>
-    <row r="270" spans="1:26">
+    <row r="270" spans="1:26" hidden="1">
       <c r="D270" s="17"/>
       <c r="E270" s="15"/>
       <c r="F270" s="15"/>
@@ -19180,7 +19181,7 @@
       <c r="Y270" s="2"/>
       <c r="Z270" s="2"/>
     </row>
-    <row r="271" spans="1:26">
+    <row r="271" spans="1:26" hidden="1">
       <c r="D271" s="17"/>
       <c r="E271" s="15"/>
       <c r="F271" s="15"/>
@@ -19207,7 +19208,7 @@
       <c r="Y271" s="2"/>
       <c r="Z271" s="2"/>
     </row>
-    <row r="272" spans="1:26">
+    <row r="272" spans="1:26" hidden="1">
       <c r="D272" s="17"/>
       <c r="E272" s="15"/>
       <c r="F272" s="15"/>
@@ -19234,7 +19235,7 @@
       <c r="Y272" s="2"/>
       <c r="Z272" s="2"/>
     </row>
-    <row r="273" spans="1:26">
+    <row r="273" spans="1:26" hidden="1">
       <c r="A273" s="51"/>
       <c r="B273" s="51"/>
       <c r="D273" s="17"/>
@@ -19263,7 +19264,7 @@
       <c r="Y273" s="2"/>
       <c r="Z273" s="2"/>
     </row>
-    <row r="274" spans="1:26">
+    <row r="274" spans="1:26" hidden="1">
       <c r="D274" s="17"/>
       <c r="E274" s="15"/>
       <c r="F274" s="15"/>
@@ -19290,7 +19291,7 @@
       <c r="Y274" s="2"/>
       <c r="Z274" s="2"/>
     </row>
-    <row r="275" spans="1:26">
+    <row r="275" spans="1:26" hidden="1">
       <c r="D275" s="17"/>
       <c r="E275" s="15"/>
       <c r="F275" s="15"/>
@@ -19317,7 +19318,7 @@
       <c r="Y275" s="2"/>
       <c r="Z275" s="2"/>
     </row>
-    <row r="276" spans="1:26">
+    <row r="276" spans="1:26" hidden="1">
       <c r="D276" s="17"/>
       <c r="E276" s="15"/>
       <c r="F276" s="15"/>
@@ -19344,7 +19345,7 @@
       <c r="Y276" s="2"/>
       <c r="Z276" s="2"/>
     </row>
-    <row r="277" spans="1:26">
+    <row r="277" spans="1:26" hidden="1">
       <c r="D277" s="17"/>
       <c r="E277" s="15"/>
       <c r="F277" s="15"/>
@@ -19371,7 +19372,7 @@
       <c r="Y277" s="2"/>
       <c r="Z277" s="2"/>
     </row>
-    <row r="278" spans="1:26">
+    <row r="278" spans="1:26" hidden="1">
       <c r="A278" s="51"/>
       <c r="B278" s="51"/>
       <c r="D278" s="17"/>
@@ -19400,7 +19401,7 @@
       <c r="Y278" s="2"/>
       <c r="Z278" s="2"/>
     </row>
-    <row r="279" spans="1:26">
+    <row r="279" spans="1:26" hidden="1">
       <c r="D279" s="17"/>
       <c r="E279" s="15"/>
       <c r="F279" s="15"/>
@@ -19427,7 +19428,7 @@
       <c r="Y279" s="2"/>
       <c r="Z279" s="2"/>
     </row>
-    <row r="280" spans="1:26">
+    <row r="280" spans="1:26" hidden="1">
       <c r="D280" s="17"/>
       <c r="E280" s="15"/>
       <c r="F280" s="15"/>
@@ -19454,7 +19455,7 @@
       <c r="Y280" s="2"/>
       <c r="Z280" s="2"/>
     </row>
-    <row r="281" spans="1:26">
+    <row r="281" spans="1:26" hidden="1">
       <c r="D281" s="17"/>
       <c r="E281" s="15"/>
       <c r="F281" s="15"/>
@@ -19481,7 +19482,7 @@
       <c r="Y281" s="2"/>
       <c r="Z281" s="2"/>
     </row>
-    <row r="282" spans="1:26">
+    <row r="282" spans="1:26" hidden="1">
       <c r="D282" s="17"/>
       <c r="E282" s="15"/>
       <c r="F282" s="15"/>
@@ -19508,7 +19509,7 @@
       <c r="Y282" s="2"/>
       <c r="Z282" s="2"/>
     </row>
-    <row r="283" spans="1:26">
+    <row r="283" spans="1:26" hidden="1">
       <c r="A283" s="51"/>
       <c r="B283" s="51"/>
       <c r="D283" s="17"/>
@@ -19537,7 +19538,7 @@
       <c r="Y283" s="2"/>
       <c r="Z283" s="2"/>
     </row>
-    <row r="284" spans="1:26">
+    <row r="284" spans="1:26" hidden="1">
       <c r="D284" s="17"/>
       <c r="E284" s="15"/>
       <c r="F284" s="15"/>
@@ -19564,7 +19565,7 @@
       <c r="Y284" s="2"/>
       <c r="Z284" s="2"/>
     </row>
-    <row r="285" spans="1:26">
+    <row r="285" spans="1:26" hidden="1">
       <c r="D285" s="17"/>
       <c r="E285" s="15"/>
       <c r="F285" s="15"/>
@@ -19591,7 +19592,7 @@
       <c r="Y285" s="2"/>
       <c r="Z285" s="2"/>
     </row>
-    <row r="286" spans="1:26">
+    <row r="286" spans="1:26" hidden="1">
       <c r="D286" s="17"/>
       <c r="E286" s="15"/>
       <c r="F286" s="15"/>
@@ -19618,7 +19619,7 @@
       <c r="Y286" s="2"/>
       <c r="Z286" s="2"/>
     </row>
-    <row r="287" spans="1:26">
+    <row r="287" spans="1:26" hidden="1">
       <c r="D287" s="17"/>
       <c r="E287" s="15"/>
       <c r="F287" s="15"/>
@@ -19645,7 +19646,7 @@
       <c r="Y287" s="2"/>
       <c r="Z287" s="2"/>
     </row>
-    <row r="288" spans="1:26">
+    <row r="288" spans="1:26" hidden="1">
       <c r="A288" s="51"/>
       <c r="B288" s="51"/>
       <c r="D288" s="17"/>
@@ -19674,7 +19675,7 @@
       <c r="Y288" s="2"/>
       <c r="Z288" s="2"/>
     </row>
-    <row r="289" spans="1:26">
+    <row r="289" spans="1:26" hidden="1">
       <c r="D289" s="17"/>
       <c r="E289" s="15"/>
       <c r="F289" s="15"/>
@@ -19701,7 +19702,7 @@
       <c r="Y289" s="2"/>
       <c r="Z289" s="2"/>
     </row>
-    <row r="290" spans="1:26">
+    <row r="290" spans="1:26" hidden="1">
       <c r="D290" s="17"/>
       <c r="E290" s="15"/>
       <c r="F290" s="15"/>
@@ -19728,7 +19729,7 @@
       <c r="Y290" s="2"/>
       <c r="Z290" s="2"/>
     </row>
-    <row r="291" spans="1:26">
+    <row r="291" spans="1:26" hidden="1">
       <c r="D291" s="17"/>
       <c r="E291" s="15"/>
       <c r="F291" s="15"/>
@@ -19755,7 +19756,7 @@
       <c r="Y291" s="2"/>
       <c r="Z291" s="2"/>
     </row>
-    <row r="292" spans="1:26">
+    <row r="292" spans="1:26" hidden="1">
       <c r="D292" s="17"/>
       <c r="E292" s="15"/>
       <c r="F292" s="15"/>
@@ -19782,7 +19783,7 @@
       <c r="Y292" s="2"/>
       <c r="Z292" s="2"/>
     </row>
-    <row r="293" spans="1:26">
+    <row r="293" spans="1:26" hidden="1">
       <c r="A293" s="51"/>
       <c r="B293" s="51"/>
       <c r="D293" s="17"/>
@@ -19811,7 +19812,7 @@
       <c r="Y293" s="2"/>
       <c r="Z293" s="2"/>
     </row>
-    <row r="294" spans="1:26">
+    <row r="294" spans="1:26" hidden="1">
       <c r="D294" s="17"/>
       <c r="E294" s="15"/>
       <c r="F294" s="15"/>
@@ -19838,7 +19839,7 @@
       <c r="Y294" s="2"/>
       <c r="Z294" s="2"/>
     </row>
-    <row r="295" spans="1:26">
+    <row r="295" spans="1:26" hidden="1">
       <c r="D295" s="17"/>
       <c r="E295" s="15"/>
       <c r="F295" s="15"/>
@@ -19865,7 +19866,7 @@
       <c r="Y295" s="2"/>
       <c r="Z295" s="2"/>
     </row>
-    <row r="296" spans="1:26">
+    <row r="296" spans="1:26" hidden="1">
       <c r="D296" s="17"/>
       <c r="E296" s="15"/>
       <c r="F296" s="15"/>
@@ -19892,7 +19893,7 @@
       <c r="Y296" s="2"/>
       <c r="Z296" s="2"/>
     </row>
-    <row r="297" spans="1:26">
+    <row r="297" spans="1:26" hidden="1">
       <c r="D297" s="17"/>
       <c r="E297" s="15"/>
       <c r="F297" s="15"/>
@@ -19919,7 +19920,7 @@
       <c r="Y297" s="2"/>
       <c r="Z297" s="2"/>
     </row>
-    <row r="298" spans="1:26">
+    <row r="298" spans="1:26" hidden="1">
       <c r="A298" s="51"/>
       <c r="B298" s="51"/>
       <c r="D298" s="17"/>
@@ -19948,7 +19949,7 @@
       <c r="Y298" s="2"/>
       <c r="Z298" s="2"/>
     </row>
-    <row r="299" spans="1:26">
+    <row r="299" spans="1:26" hidden="1">
       <c r="D299" s="17"/>
       <c r="E299" s="15"/>
       <c r="F299" s="15"/>
@@ -19975,7 +19976,7 @@
       <c r="Y299" s="2"/>
       <c r="Z299" s="2"/>
     </row>
-    <row r="300" spans="1:26">
+    <row r="300" spans="1:26" hidden="1">
       <c r="D300" s="17"/>
       <c r="E300" s="15"/>
       <c r="F300" s="15"/>
@@ -20002,7 +20003,7 @@
       <c r="Y300" s="2"/>
       <c r="Z300" s="2"/>
     </row>
-    <row r="301" spans="1:26">
+    <row r="301" spans="1:26" hidden="1">
       <c r="D301" s="17"/>
       <c r="E301" s="15"/>
       <c r="F301" s="15"/>
@@ -20029,7 +20030,7 @@
       <c r="Y301" s="2"/>
       <c r="Z301" s="2"/>
     </row>
-    <row r="302" spans="1:26">
+    <row r="302" spans="1:26" hidden="1">
       <c r="D302" s="17"/>
       <c r="E302" s="15"/>
       <c r="F302" s="15"/>
@@ -20056,7 +20057,7 @@
       <c r="Y302" s="2"/>
       <c r="Z302" s="2"/>
     </row>
-    <row r="303" spans="1:26">
+    <row r="303" spans="1:26" hidden="1">
       <c r="A303" s="51"/>
       <c r="B303" s="51"/>
       <c r="D303" s="17"/>
@@ -20085,7 +20086,7 @@
       <c r="Y303" s="2"/>
       <c r="Z303" s="2"/>
     </row>
-    <row r="304" spans="1:26">
+    <row r="304" spans="1:26" hidden="1">
       <c r="D304" s="17"/>
       <c r="E304" s="15"/>
       <c r="F304" s="15"/>
@@ -20112,7 +20113,7 @@
       <c r="Y304" s="2"/>
       <c r="Z304" s="2"/>
     </row>
-    <row r="305" spans="1:26">
+    <row r="305" spans="1:26" hidden="1">
       <c r="D305" s="17"/>
       <c r="E305" s="15"/>
       <c r="F305" s="15"/>
@@ -20139,7 +20140,7 @@
       <c r="Y305" s="2"/>
       <c r="Z305" s="2"/>
     </row>
-    <row r="306" spans="1:26">
+    <row r="306" spans="1:26" hidden="1">
       <c r="D306" s="17"/>
       <c r="E306" s="15"/>
       <c r="F306" s="15"/>
@@ -20166,7 +20167,7 @@
       <c r="Y306" s="2"/>
       <c r="Z306" s="2"/>
     </row>
-    <row r="307" spans="1:26">
+    <row r="307" spans="1:26" hidden="1">
       <c r="D307" s="17"/>
       <c r="E307" s="15"/>
       <c r="F307" s="15"/>
@@ -20193,7 +20194,7 @@
       <c r="Y307" s="2"/>
       <c r="Z307" s="2"/>
     </row>
-    <row r="308" spans="1:26">
+    <row r="308" spans="1:26" hidden="1">
       <c r="A308" s="51"/>
       <c r="B308" s="51"/>
       <c r="D308" s="17"/>
@@ -20222,7 +20223,7 @@
       <c r="Y308" s="2"/>
       <c r="Z308" s="2"/>
     </row>
-    <row r="309" spans="1:26">
+    <row r="309" spans="1:26" hidden="1">
       <c r="D309" s="17"/>
       <c r="E309" s="15"/>
       <c r="F309" s="15"/>
@@ -20249,7 +20250,7 @@
       <c r="Y309" s="2"/>
       <c r="Z309" s="2"/>
     </row>
-    <row r="310" spans="1:26">
+    <row r="310" spans="1:26" hidden="1">
       <c r="D310" s="17"/>
       <c r="E310" s="15"/>
       <c r="F310" s="15"/>
@@ -20276,7 +20277,7 @@
       <c r="Y310" s="2"/>
       <c r="Z310" s="2"/>
     </row>
-    <row r="311" spans="1:26">
+    <row r="311" spans="1:26" hidden="1">
       <c r="D311" s="17"/>
       <c r="E311" s="15"/>
       <c r="F311" s="15"/>
@@ -20303,7 +20304,7 @@
       <c r="Y311" s="2"/>
       <c r="Z311" s="2"/>
     </row>
-    <row r="312" spans="1:26">
+    <row r="312" spans="1:26" hidden="1">
       <c r="D312" s="17"/>
       <c r="E312" s="15"/>
       <c r="F312" s="15"/>
@@ -20330,7 +20331,7 @@
       <c r="Y312" s="2"/>
       <c r="Z312" s="2"/>
     </row>
-    <row r="313" spans="1:26">
+    <row r="313" spans="1:26" hidden="1">
       <c r="A313" s="51"/>
       <c r="B313" s="51"/>
       <c r="D313" s="17"/>
@@ -20359,7 +20360,7 @@
       <c r="Y313" s="2"/>
       <c r="Z313" s="2"/>
     </row>
-    <row r="314" spans="1:26">
+    <row r="314" spans="1:26" hidden="1">
       <c r="D314" s="17"/>
       <c r="E314" s="15"/>
       <c r="F314" s="15"/>
@@ -20386,7 +20387,7 @@
       <c r="Y314" s="2"/>
       <c r="Z314" s="2"/>
     </row>
-    <row r="315" spans="1:26">
+    <row r="315" spans="1:26" hidden="1">
       <c r="D315" s="17"/>
       <c r="E315" s="15"/>
       <c r="F315" s="15"/>
@@ -20413,7 +20414,7 @@
       <c r="Y315" s="2"/>
       <c r="Z315" s="2"/>
     </row>
-    <row r="316" spans="1:26">
+    <row r="316" spans="1:26" hidden="1">
       <c r="D316" s="17"/>
       <c r="E316" s="15"/>
       <c r="F316" s="15"/>
@@ -20440,7 +20441,7 @@
       <c r="Y316" s="2"/>
       <c r="Z316" s="2"/>
     </row>
-    <row r="317" spans="1:26">
+    <row r="317" spans="1:26" hidden="1">
       <c r="D317" s="17"/>
       <c r="E317" s="15"/>
       <c r="F317" s="15"/>
@@ -20467,7 +20468,7 @@
       <c r="Y317" s="2"/>
       <c r="Z317" s="2"/>
     </row>
-    <row r="318" spans="1:26">
+    <row r="318" spans="1:26" hidden="1">
       <c r="A318" s="51"/>
       <c r="B318" s="51"/>
       <c r="D318" s="17"/>
@@ -20496,7 +20497,7 @@
       <c r="Y318" s="2"/>
       <c r="Z318" s="2"/>
     </row>
-    <row r="319" spans="1:26">
+    <row r="319" spans="1:26" hidden="1">
       <c r="D319" s="17"/>
       <c r="E319" s="15"/>
       <c r="F319" s="15"/>
@@ -20523,7 +20524,7 @@
       <c r="Y319" s="2"/>
       <c r="Z319" s="2"/>
     </row>
-    <row r="320" spans="1:26">
+    <row r="320" spans="1:26" hidden="1">
       <c r="D320" s="17"/>
       <c r="E320" s="15"/>
       <c r="F320" s="15"/>
@@ -20550,7 +20551,7 @@
       <c r="Y320" s="2"/>
       <c r="Z320" s="2"/>
     </row>
-    <row r="321" spans="1:26">
+    <row r="321" spans="1:26" hidden="1">
       <c r="D321" s="17"/>
       <c r="E321" s="15"/>
       <c r="F321" s="15"/>
@@ -20577,7 +20578,7 @@
       <c r="Y321" s="2"/>
       <c r="Z321" s="2"/>
     </row>
-    <row r="322" spans="1:26">
+    <row r="322" spans="1:26" hidden="1">
       <c r="D322" s="17"/>
       <c r="E322" s="15"/>
       <c r="F322" s="15"/>
@@ -20604,7 +20605,7 @@
       <c r="Y322" s="2"/>
       <c r="Z322" s="2"/>
     </row>
-    <row r="323" spans="1:26">
+    <row r="323" spans="1:26" hidden="1">
       <c r="A323" s="51"/>
       <c r="B323" s="51"/>
       <c r="D323" s="17"/>
@@ -20633,7 +20634,7 @@
       <c r="Y323" s="2"/>
       <c r="Z323" s="2"/>
     </row>
-    <row r="324" spans="1:26">
+    <row r="324" spans="1:26" hidden="1">
       <c r="D324" s="17"/>
       <c r="E324" s="15"/>
       <c r="F324" s="15"/>
@@ -20660,7 +20661,7 @@
       <c r="Y324" s="2"/>
       <c r="Z324" s="2"/>
     </row>
-    <row r="325" spans="1:26">
+    <row r="325" spans="1:26" hidden="1">
       <c r="D325" s="17"/>
       <c r="E325" s="15"/>
       <c r="F325" s="15"/>
@@ -20687,7 +20688,7 @@
       <c r="Y325" s="2"/>
       <c r="Z325" s="2"/>
     </row>
-    <row r="326" spans="1:26">
+    <row r="326" spans="1:26" hidden="1">
       <c r="D326" s="17"/>
       <c r="E326" s="15"/>
       <c r="F326" s="15"/>
@@ -20714,7 +20715,7 @@
       <c r="Y326" s="2"/>
       <c r="Z326" s="2"/>
     </row>
-    <row r="327" spans="1:26">
+    <row r="327" spans="1:26" hidden="1">
       <c r="D327" s="17"/>
       <c r="E327" s="15"/>
       <c r="F327" s="15"/>
@@ -20741,7 +20742,7 @@
       <c r="Y327" s="2"/>
       <c r="Z327" s="2"/>
     </row>
-    <row r="328" spans="1:26">
+    <row r="328" spans="1:26" hidden="1">
       <c r="A328" s="51"/>
       <c r="B328" s="51"/>
       <c r="D328" s="17"/>
@@ -20770,7 +20771,7 @@
       <c r="Y328" s="2"/>
       <c r="Z328" s="2"/>
     </row>
-    <row r="329" spans="1:26">
+    <row r="329" spans="1:26" hidden="1">
       <c r="D329" s="17"/>
       <c r="E329" s="15"/>
       <c r="F329" s="15"/>
@@ -20797,7 +20798,7 @@
       <c r="Y329" s="2"/>
       <c r="Z329" s="2"/>
     </row>
-    <row r="330" spans="1:26">
+    <row r="330" spans="1:26" hidden="1">
       <c r="D330" s="17"/>
       <c r="E330" s="15"/>
       <c r="F330" s="15"/>
@@ -20824,7 +20825,7 @@
       <c r="Y330" s="2"/>
       <c r="Z330" s="2"/>
     </row>
-    <row r="331" spans="1:26">
+    <row r="331" spans="1:26" hidden="1">
       <c r="A331">
         <v>122</v>
       </c>
@@ -20900,7 +20901,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O333" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:O333" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="11">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="M86" r:id="rId1" xr:uid="{954017CD-E028-47AD-880B-D994F42943E3}"/>
     <hyperlink ref="M87" r:id="rId2" xr:uid="{F643B520-F58D-4BD6-B634-4474D947E197}"/>
@@ -22260,8 +22267,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:M136"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M1048576"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -22673,8 +22680,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="109">
-        <f>Aufgabenkatalog!L9</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="109"/>
       <c r="J9" s="109"/>
@@ -23158,7 +23164,7 @@
       </c>
       <c r="M19" s="109" t="str">
         <f>IF(Aufgabenkatalog!C19="Ja","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="20" spans="1:13" hidden="1">
@@ -23487,7 +23493,7 @@
       </c>
       <c r="M26" s="109" t="str">
         <f>IF(Aufgabenkatalog!C26="Ja","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="27" spans="1:13" hidden="1">
@@ -23722,7 +23728,7 @@
       </c>
       <c r="M31" s="109" t="str">
         <f>IF(Aufgabenkatalog!C31="Ja","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -23816,7 +23822,7 @@
       </c>
       <c r="M33" s="109" t="str">
         <f>IF(Aufgabenkatalog!C33="Ja","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="34" spans="1:13" hidden="1">
@@ -23957,7 +23963,7 @@
       </c>
       <c r="M36" s="109" t="str">
         <f>IF(Aufgabenkatalog!C36="Ja","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="37" spans="1:13">
@@ -25696,7 +25702,7 @@
       </c>
       <c r="M73" s="109" t="str">
         <f>IF(Aufgabenkatalog!C73="Ja","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="74" spans="1:13" hidden="1">
@@ -25790,7 +25796,7 @@
       </c>
       <c r="M75" s="109" t="str">
         <f>IF(Aufgabenkatalog!C75="Ja","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="76" spans="1:13" hidden="1">
@@ -25837,7 +25843,7 @@
       </c>
       <c r="M76" s="109" t="str">
         <f>IF(Aufgabenkatalog!C76="Ja","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="77" spans="1:13" hidden="1">
@@ -25884,7 +25890,7 @@
       </c>
       <c r="M77" s="109" t="str">
         <f>IF(Aufgabenkatalog!C77="Ja","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="78" spans="1:13" hidden="1">
@@ -25931,7 +25937,7 @@
       </c>
       <c r="M78" s="109" t="str">
         <f>IF(Aufgabenkatalog!C78="Ja","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="79" spans="1:13" hidden="1">
@@ -25978,7 +25984,7 @@
       </c>
       <c r="M79" s="109" t="str">
         <f>IF(Aufgabenkatalog!C79="Ja","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="80" spans="1:13" hidden="1">
@@ -26119,7 +26125,7 @@
       </c>
       <c r="M82" s="109" t="str">
         <f>IF(Aufgabenkatalog!C82="Ja","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="83" spans="1:13">
@@ -26354,7 +26360,7 @@
       </c>
       <c r="M87" s="109" t="str">
         <f>IF(Aufgabenkatalog!C87="Ja","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="88" spans="1:13" hidden="1">
@@ -26401,7 +26407,7 @@
       </c>
       <c r="M88" s="109" t="str">
         <f>IF(Aufgabenkatalog!C88="Ja","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="89" spans="1:13" hidden="1">
@@ -26448,7 +26454,7 @@
       </c>
       <c r="M89" s="109" t="str">
         <f>IF(Aufgabenkatalog!C89="Ja","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="90" spans="1:13" hidden="1">
@@ -26542,7 +26548,7 @@
       </c>
       <c r="M91" s="109" t="str">
         <f>IF(Aufgabenkatalog!C91="Ja","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="92" spans="1:13" hidden="1">
@@ -26589,7 +26595,7 @@
       </c>
       <c r="M92" s="109" t="str">
         <f>IF(Aufgabenkatalog!C92="Ja","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="93" spans="1:13" hidden="1">
@@ -26683,7 +26689,7 @@
       </c>
       <c r="M94" s="109" t="str">
         <f>IF(Aufgabenkatalog!C94="Ja","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="95" spans="1:13" hidden="1">
@@ -26871,7 +26877,7 @@
       </c>
       <c r="M98" s="109" t="str">
         <f>IF(Aufgabenkatalog!C98="Ja","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="99" spans="1:13" hidden="1">
@@ -26918,7 +26924,7 @@
       </c>
       <c r="M99" s="109" t="str">
         <f>IF(Aufgabenkatalog!C99="Ja","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="100" spans="1:13" hidden="1">
@@ -27059,7 +27065,7 @@
       </c>
       <c r="M102" s="109" t="str">
         <f>IF(Aufgabenkatalog!C102="Ja","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="103" spans="1:13" hidden="1">
@@ -27106,7 +27112,7 @@
       </c>
       <c r="M103" s="109" t="str">
         <f>IF(Aufgabenkatalog!C103="Ja","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="104" spans="1:13" hidden="1">
@@ -27482,7 +27488,7 @@
       </c>
       <c r="M111" s="109" t="str">
         <f>IF(Aufgabenkatalog!C111="Ja","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="112" spans="1:13" hidden="1">
@@ -27529,7 +27535,7 @@
       </c>
       <c r="M112" s="109" t="str">
         <f>IF(Aufgabenkatalog!C112="Ja","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="113" spans="1:13" hidden="1">
@@ -27576,7 +27582,7 @@
       </c>
       <c r="M113" s="109" t="str">
         <f>IF(Aufgabenkatalog!C113="Ja","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="114" spans="1:13">
@@ -27858,7 +27864,7 @@
       </c>
       <c r="M119" s="109" t="str">
         <f>IF(Aufgabenkatalog!C119="Ja","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="120" spans="1:13" hidden="1">
@@ -27905,7 +27911,7 @@
       </c>
       <c r="M120" s="109" t="str">
         <f>IF(Aufgabenkatalog!C120="Ja","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="121" spans="1:13">
@@ -28466,7 +28472,7 @@
       </c>
       <c r="M132" s="109" t="str">
         <f>IF(Aufgabenkatalog!C132="Ja","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="133" spans="1:13">
@@ -28606,7 +28612,7 @@
       </c>
       <c r="M135" s="109" t="str">
         <f>IF(Aufgabenkatalog!C135="Ja","true","false")</f>
-        <v>true</v>
+        <v>false</v>
       </c>
     </row>
     <row r="136" spans="1:13" hidden="1">

</xml_diff>